<commit_message>
major schematic change, PCB not yet updated
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\Simple-GPSDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E139557-3D37-4248-B29B-86BC246BE9FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE90F9CE-56D2-4065-9631-5A8954DE1E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35775" yWindow="2865" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="151">
   <si>
     <t>Qty</t>
   </si>
@@ -315,9 +315,6 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>8MHz</t>
-  </si>
-  <si>
     <t>SOT-23-6</t>
   </si>
   <si>
@@ -408,9 +405,6 @@
     <t>External Enclosure Mount</t>
   </si>
   <si>
-    <t>NX8045GB-8.000000MHZ</t>
-  </si>
-  <si>
     <t>PTS645SK50SMTR92 LFS</t>
   </si>
   <si>
@@ -432,15 +426,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>10.0000 MHz</t>
-  </si>
-  <si>
-    <t>McCoy OSC92-100B</t>
-  </si>
-  <si>
-    <t>OCXO</t>
-  </si>
-  <si>
     <t>Enclosure</t>
   </si>
   <si>
@@ -472,6 +457,27 @@
   </si>
   <si>
     <t>1455Q1601</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>10MHz</t>
+  </si>
+  <si>
+    <t>NV47M1008</t>
+  </si>
+  <si>
+    <t>CO-08</t>
+  </si>
+  <si>
+    <t>16MHz</t>
+  </si>
+  <si>
+    <t>TSX-3225 16.0000MF09Z-AC0</t>
+  </si>
+  <si>
+    <t>4-SMD</t>
   </si>
 </sst>
 </file>
@@ -856,15 +862,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="5"/>
   </cols>
@@ -893,12 +899,12 @@
       </c>
       <c r="H1" s="6">
         <f>SUM(G3:G54)</f>
-        <v>100.09899999999999</v>
+        <v>86.84899999999999</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -919,7 +925,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -943,10 +949,10 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" s="5">
         <v>0.22</v>
@@ -967,7 +973,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -991,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
@@ -1015,10 +1021,10 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F7" s="5">
         <v>0.44</v>
@@ -1030,19 +1036,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" s="5">
         <v>0.2</v>
@@ -1180,13 +1186,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="F14" s="5">
         <v>0.24</v>
@@ -1207,10 +1213,10 @@
         <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F15" s="5">
         <v>0.49</v>
@@ -1231,10 +1237,10 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F16" s="5">
         <v>0.76</v>
@@ -1339,19 +1345,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F21" s="5">
         <v>0</v>
@@ -1372,10 +1378,10 @@
         <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F22" s="5">
         <v>0.76</v>
@@ -1396,7 +1402,7 @@
         <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>10</v>
@@ -1420,7 +1426,7 @@
         <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>10</v>
@@ -1444,7 +1450,7 @@
         <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>10</v>
@@ -1468,7 +1474,7 @@
         <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>10</v>
@@ -1492,7 +1498,7 @@
         <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>10</v>
@@ -1516,7 +1522,7 @@
         <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>10</v>
@@ -1540,7 +1546,7 @@
         <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>10</v>
@@ -1564,7 +1570,7 @@
         <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>10</v>
@@ -1588,7 +1594,7 @@
         <v>71</v>
       </c>
       <c r="D31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>10</v>
@@ -1612,7 +1618,7 @@
         <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>78</v>
@@ -1636,7 +1642,7 @@
         <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>79</v>
@@ -1649,7 +1655,7 @@
         <v>2.02</v>
       </c>
       <c r="I33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1666,7 +1672,7 @@
         <v>87</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F34" s="5">
         <v>0.83</v>
@@ -1687,7 +1693,7 @@
         <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>89</v>
@@ -1711,10 +1717,10 @@
         <v>90</v>
       </c>
       <c r="D36" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="F36" s="5">
         <v>0.55000000000000004</v>
@@ -1738,7 +1744,7 @@
         <v>91</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F37" s="5">
         <v>0.57999999999999996</v>
@@ -1759,7 +1765,7 @@
         <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>93</v>
@@ -1783,10 +1789,10 @@
         <v>94</v>
       </c>
       <c r="D39" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="F39" s="5">
         <v>2.81</v>
@@ -1804,25 +1810,25 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="F40" s="5">
-        <v>0.56000000000000005</v>
+        <v>0.33</v>
       </c>
       <c r="G40" s="5">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1834,69 +1840,69 @@
         <v>146</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="F41" s="5">
+        <v>14.98</v>
+      </c>
+      <c r="G41" s="5">
+        <f t="shared" si="0"/>
+        <v>14.98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F42" s="5">
         <v>1.33</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G42" s="5">
         <f t="shared" si="0"/>
         <v>1.33</v>
       </c>
-      <c r="I41" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
+      <c r="I42" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>137</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>135</v>
-      </c>
-      <c r="D43" t="s">
-        <v>136</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F43" s="5">
-        <v>28</v>
-      </c>
-      <c r="G43" s="5">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
+      <c r="A43" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F44" s="5">
         <v>25</v>
@@ -1908,19 +1914,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F45" s="5">
         <v>12</v>
@@ -1950,7 +1956,7 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A43:G43"/>
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>